<commit_message>
updating which mice were not KO in ketone assay
</commit_message>
<xml_diff>
--- a/Mouse Data/Liver AMPK Ketogenic Diet/All Figures/Ketone Assay/2019-07-18 BHB Assay.xlsx
+++ b/Mouse Data/Liver AMPK Ketogenic Diet/All Figures/Ketone Assay/2019-07-18 BHB Assay.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codycousineau/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinekistler/Documents/GitHub/TissueSpecificTscKnockouts/Mouse Data/Liver AMPK Ketogenic Diet/All Figures/Ketone Assay/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331AB4F-E599-0B43-8179-0E36CF3CB617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="1920" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -356,7 +357,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -486,12 +487,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -530,7 +534,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -619,32 +622,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.308048224112832</c:v>
+                  <c:v>0.30804822411283161</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.192068771943911</c:v>
+                  <c:v>0.19206877194391114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.467512789545897</c:v>
+                  <c:v>0.46751278954589665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.301963330303042</c:v>
+                  <c:v>0.35624517107044301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.230883622504843</c:v>
+                  <c:v>0.27576895025401144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.354967525627312</c:v>
+                  <c:v>0.41536488324007559</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.156796821070648</c:v>
+                  <c:v>0.1567968210706478</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13279193477625</c:v>
+                  <c:v>0.13279193477625037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB33-2F43-A60E-A7DC0044BC69}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1371,7 +1379,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1395,14 +1409,12 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Sheet1"/>
       <sheetName val="Plate 2 - Sheet1"/>
       <sheetName val="Plate 2 - Sheet1 (1)"/>
-      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="0">
         <row r="22">
           <cell r="M22" t="str">
             <v>Early raptor</v>
@@ -1440,13 +1452,13 @@
             <v>0.46751278954589665</v>
           </cell>
           <cell r="P23">
-            <v>0.30196333030304251</v>
+            <v>0.35624517107044301</v>
           </cell>
           <cell r="Q23">
-            <v>0.23088362250484298</v>
+            <v>0.27576895025401144</v>
           </cell>
           <cell r="R23">
-            <v>0.35496752562731199</v>
+            <v>0.41536488324007559</v>
           </cell>
           <cell r="S23">
             <v>0.1567968210706478</v>
@@ -1456,6 +1468,8 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1723,11 +1737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="I237" sqref="I237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4505,14 +4519,14 @@
         <v>68.656999999999996</v>
       </c>
       <c r="O72">
-        <f t="shared" ref="O72:O83" si="4">N72/25.606</f>
+        <f t="shared" ref="O72:O77" si="4">N72/25.606</f>
         <v>2.68128563617902</v>
       </c>
       <c r="P72">
         <v>1</v>
       </c>
       <c r="Q72">
-        <f t="shared" ref="Q72:Q83" si="5">O72/P72</f>
+        <f t="shared" ref="Q72:Q80" si="5">O72/P72</f>
         <v>2.68128563617902</v>
       </c>
       <c r="R72">
@@ -7413,7 +7427,7 @@
         <v>8720</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H142" t="s">
         <v>13</v>

</xml_diff>